<commit_message>
refactor: ReadXlsx function name
</commit_message>
<xml_diff>
--- a/ProjectTemplate/bin/Debug/net8.0/Vasculhador_de_Precos.xlsx
+++ b/ProjectTemplate/bin/Debug/net8.0/Vasculhador_de_Precos.xlsx
@@ -46,6 +46,15 @@
     <x:t>Placa de Vídeo Galax NVIDIA GeForce - RTX 3050, 6GB, DDR6, 96 Bits</x:t>
   </x:si>
   <x:si>
+    <x:t>Processador AMD Ryzen 5 5600G, 3.9GHz (4.4GHz Max Turbo), AM4, Vídeo Integrado</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa Mãe Gigabyte B760M AORUS ELITE (rev. 1.0), LGA 1700, DDR5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4,4</x:t>
+  </x:si>
+  <x:si>
     <x:t>Console Playstation 5 Sony Slim, SSD 1TB, Controle Sem Fio Dualsense, Edição Digital, Branco, Returnal E Ratchet E Clank</x:t>
   </x:si>
   <x:si>
@@ -58,19 +67,28 @@
     <x:t>Placa de Vídeo RTX 3060 1-Click OC Galax NVIDIA GeForce, 12GB GDDR6, LHR, DLSS, Ray Tracing - 36NOL7MD1VOC</x:t>
   </x:si>
   <x:si>
+    <x:t>Processador AMD Ryzen 5 5600, 3.5GHz (4.4GHz Max Turbo), Cache 35MB, AM4, Sem Vídeo - 100-100000927BOX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa-Mãe AsRock B550M Steel Legend, AMD AM4 B550, DDR4 4733 OC, USB 3.2</x:t>
+  </x:si>
+  <x:si>
     <x:t>n/a</x:t>
   </x:si>
   <x:si>
     <x:t>Magazine Luiza</x:t>
   </x:si>
   <x:si>
+    <x:t>Playstation 5 Slim Digital Bundle Returnal + Ratchet &amp; Clank</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Processador AMD Ryzen 5 7600, 5.1GHz Max Turbo, Cache 38MB, AM5, 6 Núcleos, Vídeo Integrado - 100-100001015BOX</x:t>
+  </x:si>
+  <x:si>
     <x:t>5.0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Playstation 5 Slim Digital Bundle Returnal + Ratchet &amp; Clank</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4.7</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -483,13 +501,13 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B4" s="0">
-        <x:v>3799.04</x:v>
+        <x:v>1099</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
         <x:v>8</x:v>
@@ -497,16 +515,16 @@
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="A5" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B5" s="0">
-        <x:v>1639.99</x:v>
+        <x:v>1078</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
         <x:v>8</x:v>
@@ -514,10 +532,10 @@
     </x:row>
     <x:row r="6" spans="1:5">
       <x:c r="A6" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B6" s="0">
-        <x:v>0</x:v>
+        <x:v>3799.04</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
         <x:v>14</x:v>
@@ -531,13 +549,13 @@
     </x:row>
     <x:row r="7" spans="1:5">
       <x:c r="A7" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B7" s="0">
         <x:v>1639.99</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
         <x:v>15</x:v>
@@ -548,16 +566,16 @@
     </x:row>
     <x:row r="8" spans="1:5">
       <x:c r="A8" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B8" s="0">
-        <x:v>1698</x:v>
+        <x:v>799.99</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
         <x:v>8</x:v>
@@ -565,16 +583,16 @@
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="A9" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B9" s="0">
-        <x:v>1278</x:v>
+        <x:v>1612.53</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
         <x:v>8</x:v>
@@ -582,16 +600,16 @@
     </x:row>
     <x:row r="10" spans="1:5">
       <x:c r="A10" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B10" s="0">
-        <x:v>3799.04</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
         <x:v>8</x:v>
@@ -599,16 +617,16 @@
     </x:row>
     <x:row r="11" spans="1:5">
       <x:c r="A11" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B11" s="0">
-        <x:v>1639.99</x:v>
+        <x:v>3922.05</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
         <x:v>8</x:v>
@@ -616,16 +634,16 @@
     </x:row>
     <x:row r="12" spans="1:5">
       <x:c r="A12" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B12" s="0">
-        <x:v>0</x:v>
+        <x:v>1448.99</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
         <x:v>8</x:v>
@@ -633,16 +651,16 @@
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="A13" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B13" s="0">
-        <x:v>3922.05</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
         <x:v>8</x:v>

</xml_diff>